<commit_message>
Correction des doublons sur id_twitter
</commit_message>
<xml_diff>
--- a/données externes/candidats.xlsx
+++ b/données externes/candidats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoine/Documents/Études/Mastère/Cours/Enrichissement de Données et Calcul d'Indicateurs (IRT3 - B. BIRREGAH)/Projet/Twitter-Elections/données externes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura\OneDrive\Documents\MS BDAAD\Tweets Project\Twitter_Elections_Repo\Twitter-Elections\données externes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DC0272-CC8B-1141-8B2E-C2F443BFC19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EC2A71-2CA8-43A6-91E7-83556EF1D247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7100" yWindow="2340" windowWidth="25140" windowHeight="16580" xr2:uid="{1BF1B8C3-D1AE-C149-B224-859959639EAE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1BF1B8C3-D1AE-C149-B224-859959639EAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="140">
   <si>
     <t>prenom</t>
   </si>
@@ -452,6 +452,9 @@
   </si>
   <si>
     <t>date_naissance</t>
+  </si>
+  <si>
+    <t>81063019</t>
   </si>
 </sst>
 </file>
@@ -815,11 +818,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A976550-4030-124E-ABA4-A53A78C43172}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
@@ -831,7 +834,7 @@
     <col min="8" max="8" width="19.83203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -857,7 +860,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -872,7 +875,7 @@
       </c>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -898,7 +901,7 @@
         <v>43586</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -913,7 +916,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -939,7 +942,7 @@
         <v>43800</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -965,7 +968,7 @@
         <v>41214</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -988,7 +991,7 @@
         <v>40848</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1014,7 +1017,7 @@
         <v>42125</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1040,7 +1043,7 @@
         <v>40725</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1066,7 +1069,7 @@
         <v>44593</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1092,7 +1095,7 @@
         <v>43252</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1118,7 +1121,7 @@
         <v>39904</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1144,7 +1147,7 @@
         <v>42217</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1170,7 +1173,7 @@
         <v>44136</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1196,7 +1199,7 @@
         <v>40026</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1211,7 +1214,7 @@
       </c>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1237,7 +1240,7 @@
         <v>40787</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1263,7 +1266,7 @@
         <v>44652</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -1289,7 +1292,7 @@
         <v>39995</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1304,7 +1307,7 @@
       </c>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1330,7 +1333,7 @@
         <v>41579</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -1356,7 +1359,7 @@
         <v>40940</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -1370,7 +1373,7 @@
         <v>17825</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="F23" t="s">
         <v>123</v>
@@ -1382,7 +1385,7 @@
         <v>40087</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -1397,7 +1400,7 @@
       </c>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -1423,7 +1426,7 @@
         <v>41518</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -1449,7 +1452,7 @@
         <v>42491</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1464,7 +1467,7 @@
       </c>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1479,7 +1482,7 @@
       </c>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1505,7 +1508,7 @@
         <v>42186</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -1531,7 +1534,7 @@
         <v>43374</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -1546,7 +1549,7 @@
       </c>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>62</v>
       </c>
@@ -1561,7 +1564,7 @@
       </c>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1576,7 +1579,7 @@
       </c>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -1591,7 +1594,7 @@
       </c>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>66</v>
       </c>
@@ -1606,7 +1609,7 @@
       </c>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -1621,7 +1624,7 @@
       </c>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -1647,7 +1650,7 @@
         <v>40909</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -1673,7 +1676,7 @@
         <v>40057</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -1699,7 +1702,7 @@
         <v>40817</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -1725,7 +1728,7 @@
         <v>40087</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -1740,7 +1743,7 @@
       </c>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -1755,7 +1758,7 @@
       </c>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>13</v>
       </c>
@@ -1781,7 +1784,7 @@
         <v>42614</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>83</v>
       </c>
@@ -1807,7 +1810,7 @@
         <v>39508</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -1833,31 +1836,22 @@
         <v>40513</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="E3 E5:E44" numberStoredAsText="1"/>
+    <ignoredError sqref="E3 E5:E23 E24:E44" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="bff903b3-f4d0-413f-a493-3d323afbaa16">
@@ -1865,6 +1859,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2042,19 +2045,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F67799DB-C873-49D3-82F2-D94B8FA4599B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B60F110-FE9C-4A96-A6FF-9BDC69D35FD7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bff903b3-f4d0-413f-a493-3d323afbaa16"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B60F110-FE9C-4A96-A6FF-9BDC69D35FD7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F67799DB-C873-49D3-82F2-D94B8FA4599B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bff903b3-f4d0-413f-a493-3d323afbaa16"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>